<commit_message>
Spatial data and path generation in place
TO DO:
update the input parameters. Product groups should be identified with numbers.
</commit_message>
<xml_diff>
--- a/Data/SPATIAL/spatial_data.xlsx
+++ b/Data/SPATIAL/spatial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/SPATIAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="564" documentId="13_ncr:40009_{4547961E-2D41-42F0-85A9-82B80CE2B2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497E6CFF-99A3-41C7-A849-7FE98E259941}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="13_ncr:40009_{4547961E-2D41-42F0-85A9-82B80CE2B2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A117416F-FFEA-49A8-A333-9B015DED371F}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="6590" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="23400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zone_mapping" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2598,7 +2598,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -2611,9 +2611,7 @@
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2661,15 +2659,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2723,6 +2712,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <fill>
@@ -2795,11 +2793,11 @@
     <tableColumn id="1" xr3:uid="{1C81FA9B-A218-428E-9D99-3B163735CDA7}" name="zone_nr"/>
     <tableColumn id="12" xr3:uid="{C7B62B9B-D78F-4C9E-B29E-294C62D5EDC3}" name="zone_name"/>
     <tableColumn id="3" xr3:uid="{196B5265-8D2C-4B69-AB32-943B448B9E5C}" name="centroid_name"/>
-    <tableColumn id="4" xr3:uid="{05F14AA4-9D3D-4304-9767-963D4BDC03AA}" name="latitude" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7BA2B02B-7367-4F0D-8C7E-F38C69A86907}" name="longitude" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{05F14AA4-9D3D-4304-9767-963D4BDC03AA}" name="latitude" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7BA2B02B-7367-4F0D-8C7E-F38C69A86907}" name="longitude" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{41D34A41-744D-4204-8648-41EC03E8E56D}" name="lat_plot"/>
     <tableColumn id="7" xr3:uid="{333D505E-B9BC-40FF-B8D7-3392CF9071F7}" name="long_plot"/>
-    <tableColumn id="9" xr3:uid="{7A896904-1AA1-49E3-AA10-DC110DDB4EFD}" name="sea" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{7A896904-1AA1-49E3-AA10-DC110DDB4EFD}" name="sea" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{A8120715-6082-4E77-B245-67D3427B7A05}" name="road"/>
     <tableColumn id="11" xr3:uid="{428630F6-0BF6-4EC4-867C-53820282B7A4}" name="rail"/>
     <tableColumn id="8" xr3:uid="{4FA6CB03-F999-472D-A1FB-E00E603EAE1E}" name="abroad"/>
@@ -2812,9 +2810,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8A981A2D-970E-4047-9B1F-E017E4E1890A}" name="Table_1" displayName="Table_1" ref="C1:F60">
   <tableColumns count="4">
     <tableColumn id="3" xr3:uid="{2E3594F6-1493-4F41-9417-02AD3B85C1D3}" name="DistanceKM"/>
-    <tableColumn id="5" xr3:uid="{39BBD5E6-5709-4703-8D2C-2AF51853FAD6}" name="Mode" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{ECF48864-B09B-4D8C-AE0F-6FAD0ADA3614}" name="Route" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{E0688743-3C82-41D5-9DEC-1C8A146BEE3D}" name="Existing" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{39BBD5E6-5709-4703-8D2C-2AF51853FAD6}" name="Mode" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{ECF48864-B09B-4D8C-AE0F-6FAD0ADA3614}" name="Route" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E0688743-3C82-41D5-9DEC-1C8A146BEE3D}" name="Existing" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Sea-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3119,8 +3117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H555"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="N221" sqref="N221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8721,7 +8719,7 @@
         <v>610</v>
       </c>
       <c r="H215">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -8747,7 +8745,7 @@
         <v>610</v>
       </c>
       <c r="H216">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -8773,7 +8771,7 @@
         <v>610</v>
       </c>
       <c r="H217">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -8799,7 +8797,7 @@
         <v>610</v>
       </c>
       <c r="H218">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -8825,7 +8823,7 @@
         <v>610</v>
       </c>
       <c r="H219">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -8851,7 +8849,7 @@
         <v>610</v>
       </c>
       <c r="H220">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -8877,7 +8875,7 @@
         <v>610</v>
       </c>
       <c r="H221">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -8903,7 +8901,7 @@
         <v>610</v>
       </c>
       <c r="H222">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -8929,7 +8927,7 @@
         <v>610</v>
       </c>
       <c r="H223">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -8955,7 +8953,7 @@
         <v>610</v>
       </c>
       <c r="H224">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -8981,7 +8979,7 @@
         <v>610</v>
       </c>
       <c r="H225">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -9007,7 +9005,7 @@
         <v>610</v>
       </c>
       <c r="H226">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -9033,7 +9031,7 @@
         <v>610</v>
       </c>
       <c r="H227">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -9059,7 +9057,7 @@
         <v>610</v>
       </c>
       <c r="H228">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -9085,7 +9083,7 @@
         <v>610</v>
       </c>
       <c r="H229">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -9111,7 +9109,7 @@
         <v>610</v>
       </c>
       <c r="H230">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -9137,7 +9135,7 @@
         <v>610</v>
       </c>
       <c r="H231">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -9163,7 +9161,7 @@
         <v>610</v>
       </c>
       <c r="H232">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -9189,7 +9187,7 @@
         <v>610</v>
       </c>
       <c r="H233">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -17577,7 +17575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5741E99B-737E-4634-B318-C7C2DDFE7401}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -18280,8 +18278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A56265-210A-4263-A3EA-18E110BB8B83}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18319,10 +18317,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
         <v>2</v>
       </c>
       <c r="C2" s="3">
@@ -18345,10 +18343,10 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>3</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="C3" s="3">
@@ -18365,10 +18363,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="8">
         <v>23</v>
       </c>
       <c r="C4" s="3">
@@ -18385,10 +18383,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="3">
@@ -18405,10 +18403,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="8">
         <v>25</v>
       </c>
       <c r="C6" s="3">
@@ -18425,10 +18423,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="8">
         <v>4</v>
       </c>
       <c r="C7" s="3">
@@ -18465,10 +18463,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="8">
         <v>6</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9" s="3">
@@ -18485,10 +18483,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="8">
         <v>7</v>
       </c>
       <c r="C10" s="3">
@@ -18505,10 +18503,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="8">
         <v>10</v>
       </c>
       <c r="C11" s="3">
@@ -18525,7 +18523,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="8">
@@ -18545,10 +18543,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="8">
         <v>10</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="8">
         <v>12</v>
       </c>
       <c r="C13" s="3">
@@ -18563,15 +18561,15 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="13" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="8">
         <v>13</v>
       </c>
       <c r="C14" s="3">
@@ -18588,11 +18586,11 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="8">
         <v>22</v>
       </c>
-      <c r="B15" s="13">
-        <v>21</v>
+      <c r="B15" s="8">
+        <v>23</v>
       </c>
       <c r="C15" s="3">
         <v>550</v>
@@ -18621,10 +18619,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="8">
         <v>23</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="8">
         <v>24</v>
       </c>
       <c r="C16" s="3">
@@ -18650,10 +18648,10 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="8">
         <v>23</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="8">
         <v>22</v>
       </c>
       <c r="C17">
@@ -18679,10 +18677,10 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="6">
         <v>8</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="6">
         <v>22</v>
       </c>
       <c r="C18" s="5">
@@ -18708,10 +18706,10 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="A19" s="6">
         <v>8</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>7</v>
       </c>
       <c r="C19" s="5">
@@ -18737,10 +18735,10 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>1</v>
-      </c>
-      <c r="B20" s="14">
+      <c r="A20" s="6">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
         <v>8</v>
       </c>
       <c r="C20" s="5">
@@ -18766,10 +18764,10 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>1</v>
-      </c>
-      <c r="B21" s="14">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6">
         <v>5</v>
       </c>
       <c r="C21" s="5">
@@ -18795,10 +18793,10 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>1</v>
-      </c>
-      <c r="B22" s="14">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
         <v>22</v>
       </c>
       <c r="C22" s="5">
@@ -18824,10 +18822,10 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>1</v>
-      </c>
-      <c r="B23" s="14">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6">
         <v>23</v>
       </c>
       <c r="C23" s="5">
@@ -18853,10 +18851,10 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>1</v>
-      </c>
-      <c r="B24" s="14">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6">
         <v>2</v>
       </c>
       <c r="C24" s="5">
@@ -18882,10 +18880,10 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="A25" s="6">
         <v>2</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="6">
         <v>5</v>
       </c>
       <c r="C25" s="5">
@@ -18911,10 +18909,10 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="A26" s="6">
         <v>2</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="6">
         <v>3</v>
       </c>
       <c r="C26" s="5">
@@ -18940,10 +18938,10 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
+      <c r="A27" s="6">
         <v>3</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="6">
         <v>4</v>
       </c>
       <c r="C27" s="5">
@@ -18969,10 +18967,10 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="A28" s="6">
         <v>4</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="6">
         <v>5</v>
       </c>
       <c r="C28" s="5">
@@ -18998,10 +18996,10 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="6">
         <v>5</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="6">
         <v>6</v>
       </c>
       <c r="C29" s="5">
@@ -19027,10 +19025,10 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="6">
         <v>6</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="6">
         <v>7</v>
       </c>
       <c r="C30" s="5">
@@ -19056,10 +19054,10 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="6">
         <v>9</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="6">
         <v>7</v>
       </c>
       <c r="C31" s="5">
@@ -19085,10 +19083,10 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="6">
         <v>9</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="6">
         <v>8</v>
       </c>
       <c r="C32" s="5">
@@ -19114,10 +19112,10 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="A33" s="6">
         <v>9</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="6">
         <v>22</v>
       </c>
       <c r="C33" s="5">
@@ -19143,10 +19141,10 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+      <c r="A34" s="6">
         <v>9</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="6">
         <v>21</v>
       </c>
       <c r="C34" s="5">
@@ -19166,10 +19164,10 @@
       <c r="N34" s="10"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+      <c r="A35" s="6">
         <v>9</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="6">
         <v>10</v>
       </c>
       <c r="C35" s="5">
@@ -19189,10 +19187,10 @@
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+      <c r="A36" s="6">
         <v>10</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="6">
         <v>21</v>
       </c>
       <c r="C36" s="5">
@@ -19212,10 +19210,10 @@
       <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+      <c r="A37" s="6">
         <v>10</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="6">
         <v>11</v>
       </c>
       <c r="C37" s="5">
@@ -19232,10 +19230,10 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
+      <c r="A38" s="6">
         <v>11</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="6">
         <v>21</v>
       </c>
       <c r="C38" s="5">
@@ -19252,10 +19250,10 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+      <c r="A39" s="6">
         <v>11</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="6">
         <v>12</v>
       </c>
       <c r="C39" s="5">
@@ -19272,10 +19270,10 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="A40" s="6">
         <v>12</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="6">
         <v>21</v>
       </c>
       <c r="C40" s="5">
@@ -19292,10 +19290,10 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+      <c r="A41" s="6">
         <v>12</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="6">
         <v>13</v>
       </c>
       <c r="C41" s="5">
@@ -19312,10 +19310,10 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+      <c r="A42" s="6">
         <v>22</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="6">
         <v>21</v>
       </c>
       <c r="C42" s="5">
@@ -19332,10 +19330,10 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+      <c r="A43" s="6">
         <v>22</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="6">
         <v>23</v>
       </c>
       <c r="C43" s="6">

</xml_diff>

<commit_message>
Various bugfixes (mainly investment related)
Current bug is at the BassDiffusionSecondStage constraint
</commit_message>
<xml_diff>
--- a/Data/SPATIAL/spatial_data.xlsx
+++ b/Data/SPATIAL/spatial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steffejb\OneDrive - NTNU\Work\GitHub\STraM_ntnu_development\Data\SPATIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F74FBB8B-6408-4A75-B24C-CB2315E4B04F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BB88D83-FF5D-48CC-87BB-F4011D68107D}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{F74FBB8B-6408-4A75-B24C-CB2315E4B04F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6CE65D1-1196-400D-A8C8-7017D84CE7D6}"/>
   <bookViews>
-    <workbookView xWindow="14750" yWindow="350" windowWidth="28800" windowHeight="22170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14750" yWindow="350" windowWidth="28800" windowHeight="22170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zone_mapping" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="671">
   <si>
     <t>NGM_zone_nr</t>
   </si>
@@ -17504,8 +17504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5741E99B-737E-4634-B318-C7C2DDFE7401}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18012,10 +18012,13 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -18210,7 +18213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A56265-210A-4263-A3EA-18E110BB8B83}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
@@ -19669,6 +19672,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80174008b946241598c9c4dc1e838b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83c7d99240e58c9b66f78776c092749e" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -19909,24 +19929,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25E92F15-5C9E-4743-BBCA-DF2A8E467494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F11BAE-A5D0-4A24-BFFD-064A72F53DEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36DD76E4-C162-4392-939E-9C4A48CBB9A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19943,29 +19971,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F11BAE-A5D0-4A24-BFFD-064A72F53DEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25E92F15-5C9E-4743-BBCA-DF2A8E467494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>